<commit_message>
Update Practice Self Rating Tool.xlsx
</commit_message>
<xml_diff>
--- a/Practice Self Rating Tool.xlsx
+++ b/Practice Self Rating Tool.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/raving_microsoft_com1/Documents/Desktop/Partner Practice Toolkit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RaviGitLocal\Partner_Practice_Toolkit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86299BB1-1BB4-4EC7-AB7C-B917AAFB937C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535B4493-1E1B-488D-A38E-FDF654C2926C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35115" yWindow="120" windowWidth="18900" windowHeight="13485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33060" yWindow="1830" windowWidth="22695" windowHeight="13485" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Action Plan Template" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -213,9 +212,6 @@
   </si>
   <si>
     <t>ESG Domain Expertise</t>
-  </si>
-  <si>
-    <t>Community Engagement</t>
   </si>
   <si>
     <t>Product Knowledge Alignment</t>
@@ -487,6 +483,9 @@
       </rPr>
       <t xml:space="preserve"> (Copy from Practice Maturity Tool Worksheet)</t>
     </r>
+  </si>
+  <si>
+    <t>Copilot and Agentic AI proficiency</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
@@ -1133,7 +1132,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="61.5" x14ac:dyDescent="0.35">
@@ -1147,13 +1146,13 @@
         <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="46.5" x14ac:dyDescent="0.35">
@@ -1164,7 +1163,7 @@
         <v>50</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>11</v>
@@ -1193,7 +1192,7 @@
         <v>19</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="61.5" x14ac:dyDescent="0.35">
@@ -1218,7 +1217,7 @@
     </row>
     <row r="8" spans="2:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B8" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>23</v>
@@ -1230,10 +1229,10 @@
         <v>25</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1244,7 +1243,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1279,13 +1278,13 @@
         <v>31</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -1314,7 +1313,7 @@
     </row>
     <row r="14" spans="2:9" ht="76.5" x14ac:dyDescent="0.35">
       <c r="B14" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>29</v>
@@ -1329,7 +1328,7 @@
         <v>37</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1342,7 +1341,7 @@
         <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>40</v>
@@ -1386,7 +1385,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I17" s="2"/>
     </row>
@@ -1420,19 +1419,19 @@
         <v>55</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1442,19 +1441,19 @@
         <v>56</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1464,63 +1463,63 @@
         <v>57</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
     <row r="23" spans="2:9" ht="166.5" x14ac:dyDescent="0.35">
       <c r="B23" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="2:9" ht="91.5" x14ac:dyDescent="0.35">
       <c r="B24" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -1532,7 +1531,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I25" s="2"/>
     </row>
@@ -1559,7 +1558,7 @@
     </row>
     <row r="28" spans="2:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B28" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="2"/>
@@ -1571,110 +1570,110 @@
     </row>
     <row r="29" spans="2:9" ht="76.5" x14ac:dyDescent="0.35">
       <c r="B29" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="2:9" ht="61.5" x14ac:dyDescent="0.35">
       <c r="B30" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="2:9" ht="61.5" x14ac:dyDescent="0.35">
       <c r="B31" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="2:9" ht="76.5" x14ac:dyDescent="0.35">
       <c r="B32" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="2:9" ht="61.5" x14ac:dyDescent="0.35">
       <c r="B33" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -1686,7 +1685,7 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I34" s="2"/>
     </row>
@@ -1740,7 +1739,7 @@
     </row>
     <row r="40" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C40" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D40" s="12" t="e">
         <f>AVERAGE(H10,H18,H26,H35)</f>
@@ -1763,7 +1762,7 @@
     </row>
     <row r="42" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C42" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D42" s="12" t="e">
         <f>IF(AND(D40&gt;=5, D40&lt;=9), "Foundational",
@@ -1792,10 +1791,10 @@
     </row>
     <row r="46" spans="2:9" ht="189.75" x14ac:dyDescent="0.4">
       <c r="C46" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D46" s="11" t="s">
         <v>132</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1807,8 +1806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC6323A-9198-4E88-9956-8B1D9BA503FD}">
   <dimension ref="B4:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1821,16 +1820,16 @@
   <sheetData>
     <row r="4" spans="2:5" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -1853,7 +1852,7 @@
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1863,7 +1862,7 @@
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1873,13 +1872,13 @@
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="20"/>
       <c r="C10" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -1920,7 +1919,7 @@
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="20"/>
       <c r="C16" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -1985,7 +1984,7 @@
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="20"/>
       <c r="C25" s="6" t="s">
-        <v>58</v>
+        <v>140</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -1993,7 +1992,7 @@
     <row r="26" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="20"/>
       <c r="C26" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
@@ -2012,7 +2011,7 @@
     </row>
     <row r="30" spans="2:5" ht="21" x14ac:dyDescent="0.35">
       <c r="C30" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -2020,7 +2019,7 @@
     <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="20"/>
       <c r="C31" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
@@ -2028,7 +2027,7 @@
     <row r="32" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="20"/>
       <c r="C32" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -2036,7 +2035,7 @@
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="20"/>
       <c r="C33" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
@@ -2044,7 +2043,7 @@
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="20"/>
       <c r="C34" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
@@ -2052,7 +2051,7 @@
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="20"/>
       <c r="C35" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -2064,27 +2063,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65fe09e8-716e-4918-accf-ed9478271149">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA38213EED8AE445B4F84D5EF72853CF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1a6f101ec9e0d4e30167501548f36a60">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fe6154f8-a261-43c7-b4d0-ba3907e7242d" xmlns:ns3="65fe09e8-716e-4918-accf-ed9478271149" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="13bb6da802fe090b017c36dccf7b81d9" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2318,33 +2296,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CC39AF9-BBE7-432F-BB1A-D51CB595552C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="65fe09e8-716e-4918-accf-ed9478271149"/>
-    <ds:schemaRef ds:uri="fe6154f8-a261-43c7-b4d0-ba3907e7242d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04EE217D-593D-41F0-A9EE-11B35884CA33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65fe09e8-716e-4918-accf-ed9478271149">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B814E18-2C2B-46ED-A05F-D0BA89BC95C4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2364,6 +2337,32 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04EE217D-593D-41F0-A9EE-11B35884CA33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CC39AF9-BBE7-432F-BB1A-D51CB595552C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="65fe09e8-716e-4918-accf-ed9478271149"/>
+    <ds:schemaRef ds:uri="fe6154f8-a261-43c7-b4d0-ba3907e7242d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{87867195-f2b8-4ac2-b0b6-6bb73cb33afc}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>